<commit_message>
Added password checking when if microsoft remember user's password
</commit_message>
<xml_diff>
--- a/Succeed Invoices.xlsx
+++ b/Succeed Invoices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LiBo3\PycharmProjects\PythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA969673-012F-43ED-B7D0-11BEBCBDF849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F4636D-9247-43B2-B42C-AD80CBE87E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -349,7 +349,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>